<commit_message>
sprint3 final DOCs update
</commit_message>
<xml_diff>
--- a/DOCs/BurnDownTeam2Wk1Sprint3.xlsx
+++ b/DOCs/BurnDownTeam2Wk1Sprint3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AA84BA-1623-4E56-9B1D-4B93DF0601B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C967979-EF92-4346-A48B-1A2B80CFB3FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4877" yWindow="917" windowWidth="24686" windowHeight="13149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2683" yWindow="1689" windowWidth="24686" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -526,76 +526,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>37</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -721,43 +721,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>37</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.6</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.133333333333333</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.666666666666664</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.2</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.733333333333334</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.266666666666666</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.799999999999997</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.333333333333332</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.8666666666666671</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.3999999999999986</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.93333333333333</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4666666666666686</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -3463,7 +3463,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3504,16 +3504,16 @@
         <v>43570</v>
       </c>
       <c r="C2" s="3">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="1">
         <f>C2-D2</f>
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F2" s="4">
         <f>$C$2</f>
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -3527,11 +3527,11 @@
       <c r="D3" s="3"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E7" si="0">(E2+C3)-D3</f>
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F3" s="4">
         <f t="shared" ref="F3:F15" si="1">$C$2-(($C$2/15)*(A2+2))</f>
-        <v>29.6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" si="1"/>
-        <v>27.133333333333333</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -3565,11 +3565,11 @@
       <c r="D5" s="3"/>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="1"/>
-        <v>24.666666666666664</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -3583,11 +3583,11 @@
       <c r="D6" s="3"/>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="1"/>
-        <v>22.2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -3601,11 +3601,11 @@
       <c r="D7" s="3"/>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="1"/>
-        <v>19.733333333333334</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -3619,11 +3619,11 @@
       <c r="D8" s="3"/>
       <c r="E8" s="1">
         <f t="shared" ref="E8:E25" si="2">(E7+C8)-D8</f>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="1"/>
-        <v>17.266666666666666</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -3637,11 +3637,11 @@
       <c r="D9" s="3"/>
       <c r="E9" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="1"/>
-        <v>14.799999999999997</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -3655,11 +3655,11 @@
       <c r="D10" s="3"/>
       <c r="E10" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="1"/>
-        <v>12.333333333333332</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -3673,11 +3673,11 @@
       <c r="D11" s="3"/>
       <c r="E11" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="1"/>
-        <v>9.8666666666666671</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
@@ -3691,11 +3691,11 @@
       <c r="D12" s="3"/>
       <c r="E12" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="1"/>
-        <v>7.3999999999999986</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
@@ -3709,11 +3709,11 @@
       <c r="D13" s="3"/>
       <c r="E13" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="1"/>
-        <v>4.93333333333333</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
@@ -3727,11 +3727,11 @@
       <c r="D14" s="3"/>
       <c r="E14" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" si="1"/>
-        <v>2.4666666666666686</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
@@ -3745,7 +3745,7 @@
       <c r="D15" s="3"/>
       <c r="E15" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F15" s="4">
         <f t="shared" si="1"/>
@@ -3763,7 +3763,7 @@
       <c r="D16" s="3"/>
       <c r="E16" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F16" s="4">
         <v>0</v>
@@ -3780,7 +3780,7 @@
       <c r="D17" s="3"/>
       <c r="E17" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F17" s="4">
         <v>0</v>
@@ -3797,7 +3797,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F18" s="4">
         <v>0</v>
@@ -3814,7 +3814,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -3831,7 +3831,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -3848,7 +3848,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F21" s="4">
         <v>0</v>
@@ -3865,7 +3865,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F22" s="4">
         <v>0</v>
@@ -3882,7 +3882,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -3899,7 +3899,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F24" s="4">
         <f t="shared" ref="F24" si="3">$C$2-(($C$2/24)*(A23+2))</f>
@@ -3917,7 +3917,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F25" s="4">
         <f>$C$2-(($C$2/24)*(A24+1))</f>
@@ -3927,7 +3927,7 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C26" s="1">
         <f>SUM(C2:C25)</f>
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D26" s="1">
         <f>SUM(D2:D25)</f>

</xml_diff>